<commit_message>
modified:   reportmail.py 	modified:   "\345\257\204\351\200\201\351\203\265\344\273\266\351\200\232\350\250\212\351\214\204.xlsx"
</commit_message>
<xml_diff>
--- a/寄送郵件通訊錄.xlsx
+++ b/寄送郵件通訊錄.xlsx
@@ -1,31 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program\Repormail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC51E632-37B5-4545-AE43-535ABC3BD95E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20DF4AD-8DCD-4CEC-A174-52A3C7EE52FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>寄送對象</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -57,6 +66,22 @@
   </si>
   <si>
     <t>yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>備註</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>洪國瑋</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -109,9 +134,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -393,15 +421,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -423,8 +451,11 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -445,14 +476,32 @@
       </c>
       <c r="G2" t="s">
         <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{232785F9-C92A-4CA5-9FAE-CE61E5FCFFF1}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{1457F7DB-DBB3-457C-9A31-6D0B1839CB36}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modified:   "\345\257\204\351\200\201\351\203\265\344\273\266\351\200\232\350\250\212\351\214\204.xlsx" 	modified:   "\347\216\213\345\272\247\345\234\213\351\232\233\351\226\200\345\270\202\351\200\232\350\250\212\351\214\204.xlsx"
</commit_message>
<xml_diff>
--- a/寄送郵件通訊錄.xlsx
+++ b/寄送郵件通訊錄.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program\Repormail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20DF4AD-8DCD-4CEC-A174-52A3C7EE52FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94776841-A7CD-4CB3-AF70-5756AE1FC22A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
   <si>
     <t>寄送對象</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -81,8 +81,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>洪國瑋</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>鄭守利</t>
   </si>
 </sst>
 </file>
@@ -421,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
@@ -488,11 +487,22 @@
       <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
       <c r="H3" s="2" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -500,8 +510,9 @@
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{232785F9-C92A-4CA5-9FAE-CE61E5FCFFF1}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{1457F7DB-DBB3-457C-9A31-6D0B1839CB36}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{0B98E0A6-E76C-4560-BAE7-662908D7DD31}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modified:   Datamerge.py 	modified:   __pycache__/SQL_tra.cpython-312.pyc 	modified:   "\345\257\204\351\200\201\351\203\265\344\273\266\351\200\232\350\250\212\351\214\204.xlsx"
</commit_message>
<xml_diff>
--- a/寄送郵件通訊錄.xlsx
+++ b/寄送郵件通訊錄.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program\Repormail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94776841-A7CD-4CB3-AF70-5756AE1FC22A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDE3F62-B030-4DE9-8CB3-2D18E9A020EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>寄送對象</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -423,7 +423,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
@@ -503,6 +503,9 @@
       </c>
       <c r="G4" t="s">
         <v>8</v>
+      </c>
+      <c r="H4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>